<commit_message>
Commented Jar Creation Build and Adding testng.xml build to POM
</commit_message>
<xml_diff>
--- a/data/TDCN1.xlsx
+++ b/data/TDCN1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>Sno</t>
   </si>
@@ -176,29 +176,13 @@
   </si>
   <si>
     <t>02-11-1978,01-11-2005,01-11-2023</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Pass : 45</t>
-  </si>
-  <si>
-    <t>Pass : 18</t>
-  </si>
-  <si>
-    <t>1.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,50 +197,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -592,14 +532,14 @@
   <dimension ref="A1:AS2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AI10" sqref="AI10"/>
+      <selection activeCell="AQ10" sqref="AQ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="28" max="30" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="31" max="32" customWidth="true" width="38.140625" collapsed="true"/>
+    <col min="2" max="2" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="28" max="30" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="31" max="32" width="38.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -830,45 +770,12 @@
       <c r="AD2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AE2" t="e">
+      <c r="AE2" t="str">
         <f t="shared" ref="AE2" si="0">TEXT(AB2,"dd-mm-yyyy")&amp;","&amp;TEXT(AC2,"dd-mm-yyyy")&amp;","&amp;TEXT(AD2,"dd-mm-yyyy")</f>
-        <v>#VALUE!</v>
+        <v>02-11-1978,01-11-2005,01-11-2023</v>
       </c>
       <c r="AF2" t="s">
         <v>53</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>